<commit_message>
log-in test case completed
</commit_message>
<xml_diff>
--- a/coffeShop-manual-tests.xlsx
+++ b/coffeShop-manual-tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test scenarios" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="79">
   <si>
     <t>Id</t>
   </si>
@@ -211,6 +211,48 @@
   </si>
   <si>
     <t>Checking the validation of log-in form that user is able to log-in with correct and incorrect data</t>
+  </si>
+  <si>
+    <t>User should log-in if he has provided all correct data</t>
+  </si>
+  <si>
+    <t>Log in with correct data</t>
+  </si>
+  <si>
+    <t>Check if the user has access to the log-in form</t>
+  </si>
+  <si>
+    <t>Click on "Log in" button</t>
+  </si>
+  <si>
+    <t>User should be redirected to the log-in page</t>
+  </si>
+  <si>
+    <t>User is redirected on log-in page</t>
+  </si>
+  <si>
+    <t>Fill the form inputs with correct data (email, password)</t>
+  </si>
+  <si>
+    <t>Click on button "log in"</t>
+  </si>
+  <si>
+    <t>User should be redirected to the main page</t>
+  </si>
+  <si>
+    <t>Log in with incorrect data</t>
+  </si>
+  <si>
+    <t>User should be notified that he provided wrong password or email</t>
+  </si>
+  <si>
+    <t>Fill the form inputs with incorrect data (email, password)</t>
+  </si>
+  <si>
+    <t>Should display error under email input you provided "Wrong password or email"</t>
+  </si>
+  <si>
+    <t>Error "Wrong password or email" is displayed</t>
   </si>
 </sst>
 </file>
@@ -297,7 +339,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -452,12 +494,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FFC00000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -791,6 +879,21 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1331,8 +1434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:AA84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AE63" sqref="AE63"/>
+    <sheetView topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U81" sqref="U81:W84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3947,14 +4050,1602 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M35" sqref="M35:P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="U2" s="4"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="33"/>
+    </row>
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="29">
+        <v>1</v>
+      </c>
+      <c r="C3" s="29">
+        <v>1</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+      <c r="T3" s="34"/>
+      <c r="U3" s="34"/>
+      <c r="V3" s="34"/>
+      <c r="W3" s="34"/>
+      <c r="X3" s="34"/>
+      <c r="Y3" s="34"/>
+      <c r="Z3" s="34"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="34"/>
+      <c r="T4" s="34"/>
+      <c r="U4" s="34"/>
+      <c r="V4" s="34"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="34"/>
+      <c r="X5" s="34"/>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
+      <c r="S6" s="34"/>
+      <c r="T6" s="34"/>
+      <c r="U6" s="34"/>
+      <c r="V6" s="34"/>
+      <c r="W6" s="34"/>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="34"/>
+      <c r="Z6" s="34"/>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="63"/>
+      <c r="S7" s="64"/>
+      <c r="T7" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="U7" s="41"/>
+      <c r="V7" s="42"/>
+      <c r="W7" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="42"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="65"/>
+      <c r="R8" s="66"/>
+      <c r="S8" s="67"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="44"/>
+      <c r="Y8" s="44"/>
+      <c r="Z8" s="45"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="65"/>
+      <c r="R9" s="66"/>
+      <c r="S9" s="67"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="44"/>
+      <c r="Y9" s="44"/>
+      <c r="Z9" s="45"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37"/>
+      <c r="O10" s="37"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="68"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="46"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="46"/>
+      <c r="X10" s="47"/>
+      <c r="Y10" s="47"/>
+      <c r="Z10" s="48"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="60"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="19"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="53"/>
+      <c r="Q11" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="83"/>
+      <c r="S11" s="84"/>
+      <c r="T11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U11" s="19"/>
+      <c r="V11" s="20"/>
+      <c r="W11" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="20"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="56"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="87"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="21"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+      <c r="Z12" s="23"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="56"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="86"/>
+      <c r="S13" s="87"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="22"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+      <c r="Z13" s="23"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="62"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="58"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="59"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="89"/>
+      <c r="S14" s="90"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="24"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="25"/>
+      <c r="Z14" s="26"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="41"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="N15" s="72"/>
+      <c r="O15" s="72"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="R15" s="63"/>
+      <c r="S15" s="64"/>
+      <c r="T15" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="U15" s="41"/>
+      <c r="V15" s="42"/>
+      <c r="W15" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="42"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="75"/>
+      <c r="O16" s="75"/>
+      <c r="P16" s="76"/>
+      <c r="Q16" s="65"/>
+      <c r="R16" s="66"/>
+      <c r="S16" s="67"/>
+      <c r="T16" s="43"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="44"/>
+      <c r="Y16" s="44"/>
+      <c r="Z16" s="45"/>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B17" s="81"/>
+      <c r="C17" s="81"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="75"/>
+      <c r="O17" s="75"/>
+      <c r="P17" s="76"/>
+      <c r="Q17" s="65"/>
+      <c r="R17" s="66"/>
+      <c r="S17" s="67"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="44"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="44"/>
+      <c r="Y17" s="44"/>
+      <c r="Z17" s="45"/>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B18" s="82"/>
+      <c r="C18" s="82"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="77"/>
+      <c r="N18" s="78"/>
+      <c r="O18" s="78"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="68"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="46"/>
+      <c r="U18" s="47"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="46"/>
+      <c r="X18" s="47"/>
+      <c r="Y18" s="47"/>
+      <c r="Z18" s="48"/>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="X19" s="19"/>
+      <c r="Y19" s="19"/>
+      <c r="Z19" s="20"/>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="21"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+      <c r="Z20" s="23"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="21"/>
+      <c r="X21" s="22"/>
+      <c r="Y21" s="22"/>
+      <c r="Z21" s="23"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="24"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="26"/>
+    </row>
+    <row r="23" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B23" s="36"/>
+      <c r="C23" s="36"/>
+      <c r="D23" s="36"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="N23" s="37"/>
+      <c r="O23" s="37"/>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="R23" s="37"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="U23" s="36"/>
+      <c r="V23" s="36"/>
+      <c r="W23" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X23" s="41"/>
+      <c r="Y23" s="41"/>
+      <c r="Z23" s="42"/>
+    </row>
+    <row r="24" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B24" s="36"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="37"/>
+      <c r="N24" s="37"/>
+      <c r="O24" s="37"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="37"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="44"/>
+      <c r="Y24" s="44"/>
+      <c r="Z24" s="45"/>
+    </row>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="37"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="37"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="37"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="36"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="44"/>
+      <c r="Y25" s="44"/>
+      <c r="Z25" s="45"/>
+    </row>
+    <row r="26" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="113"/>
+      <c r="C26" s="113"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="113"/>
+      <c r="F26" s="113"/>
+      <c r="G26" s="113"/>
+      <c r="H26" s="113"/>
+      <c r="I26" s="113"/>
+      <c r="J26" s="113"/>
+      <c r="K26" s="113"/>
+      <c r="L26" s="113"/>
+      <c r="M26" s="114"/>
+      <c r="N26" s="114"/>
+      <c r="O26" s="114"/>
+      <c r="P26" s="114"/>
+      <c r="Q26" s="114"/>
+      <c r="R26" s="114"/>
+      <c r="S26" s="114"/>
+      <c r="T26" s="113"/>
+      <c r="U26" s="113"/>
+      <c r="V26" s="113"/>
+      <c r="W26" s="115"/>
+      <c r="X26" s="116"/>
+      <c r="Y26" s="116"/>
+      <c r="Z26" s="117"/>
+    </row>
+    <row r="27" spans="2:26" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="61"/>
+      <c r="C27" s="61">
+        <v>2</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" s="23"/>
+      <c r="F27" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="N27" s="62"/>
+      <c r="O27" s="62"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="62"/>
+      <c r="R27" s="62"/>
+      <c r="S27" s="62"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="62"/>
+    </row>
+    <row r="28" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="34"/>
+      <c r="L28" s="34"/>
+      <c r="M28" s="34"/>
+      <c r="N28" s="34"/>
+      <c r="O28" s="34"/>
+      <c r="P28" s="34"/>
+      <c r="Q28" s="34"/>
+      <c r="R28" s="34"/>
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+      <c r="U28" s="34"/>
+      <c r="V28" s="34"/>
+      <c r="W28" s="34"/>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="34"/>
+      <c r="Z28" s="34"/>
+    </row>
+    <row r="29" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
+      <c r="O29" s="34"/>
+      <c r="P29" s="34"/>
+      <c r="Q29" s="34"/>
+      <c r="R29" s="34"/>
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="34"/>
+      <c r="W29" s="34"/>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="34"/>
+      <c r="Z29" s="34"/>
+    </row>
+    <row r="30" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34"/>
+      <c r="N30" s="34"/>
+      <c r="O30" s="34"/>
+      <c r="P30" s="34"/>
+      <c r="Q30" s="34"/>
+      <c r="R30" s="34"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="34"/>
+      <c r="W30" s="34"/>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="34"/>
+      <c r="Z30" s="34"/>
+    </row>
+    <row r="31" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
+      <c r="J31" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="K31" s="41"/>
+      <c r="L31" s="42"/>
+      <c r="M31" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="N31" s="37"/>
+      <c r="O31" s="37"/>
+      <c r="P31" s="37"/>
+      <c r="Q31" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="R31" s="63"/>
+      <c r="S31" s="64"/>
+      <c r="T31" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="U31" s="41"/>
+      <c r="V31" s="42"/>
+      <c r="W31" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X31" s="41"/>
+      <c r="Y31" s="41"/>
+      <c r="Z31" s="42"/>
+    </row>
+    <row r="32" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B32" s="81"/>
+      <c r="C32" s="81"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="45"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44"/>
+      <c r="H32" s="44"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="44"/>
+      <c r="L32" s="45"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="37"/>
+      <c r="O32" s="37"/>
+      <c r="P32" s="37"/>
+      <c r="Q32" s="65"/>
+      <c r="R32" s="66"/>
+      <c r="S32" s="67"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="44"/>
+      <c r="V32" s="45"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="44"/>
+      <c r="Y32" s="44"/>
+      <c r="Z32" s="45"/>
+    </row>
+    <row r="33" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B33" s="81"/>
+      <c r="C33" s="81"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
+      <c r="J33" s="43"/>
+      <c r="K33" s="44"/>
+      <c r="L33" s="45"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="37"/>
+      <c r="O33" s="37"/>
+      <c r="P33" s="37"/>
+      <c r="Q33" s="65"/>
+      <c r="R33" s="66"/>
+      <c r="S33" s="67"/>
+      <c r="T33" s="43"/>
+      <c r="U33" s="44"/>
+      <c r="V33" s="45"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="44"/>
+      <c r="Y33" s="44"/>
+      <c r="Z33" s="45"/>
+    </row>
+    <row r="34" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B34" s="82"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="48"/>
+      <c r="J34" s="46"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="48"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="37"/>
+      <c r="O34" s="37"/>
+      <c r="P34" s="37"/>
+      <c r="Q34" s="68"/>
+      <c r="R34" s="69"/>
+      <c r="S34" s="70"/>
+      <c r="T34" s="46"/>
+      <c r="U34" s="47"/>
+      <c r="V34" s="48"/>
+      <c r="W34" s="46"/>
+      <c r="X34" s="47"/>
+      <c r="Y34" s="47"/>
+      <c r="Z34" s="48"/>
+    </row>
+    <row r="35" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K35" s="19"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="R35" s="83"/>
+      <c r="S35" s="84"/>
+      <c r="T35" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="U35" s="19"/>
+      <c r="V35" s="20"/>
+      <c r="W35" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="19"/>
+      <c r="Z35" s="20"/>
+    </row>
+    <row r="36" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="54"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="85"/>
+      <c r="R36" s="86"/>
+      <c r="S36" s="87"/>
+      <c r="T36" s="21"/>
+      <c r="U36" s="22"/>
+      <c r="V36" s="23"/>
+      <c r="W36" s="21"/>
+      <c r="X36" s="22"/>
+      <c r="Y36" s="22"/>
+      <c r="Z36" s="23"/>
+    </row>
+    <row r="37" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="23"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="23"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="54"/>
+      <c r="N37" s="55"/>
+      <c r="O37" s="55"/>
+      <c r="P37" s="56"/>
+      <c r="Q37" s="85"/>
+      <c r="R37" s="86"/>
+      <c r="S37" s="87"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="22"/>
+      <c r="V37" s="23"/>
+      <c r="W37" s="21"/>
+      <c r="X37" s="22"/>
+      <c r="Y37" s="22"/>
+      <c r="Z37" s="23"/>
+    </row>
+    <row r="38" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="24"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="26"/>
+      <c r="M38" s="57"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="58"/>
+      <c r="P38" s="59"/>
+      <c r="Q38" s="88"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="90"/>
+      <c r="T38" s="24"/>
+      <c r="U38" s="25"/>
+      <c r="V38" s="26"/>
+      <c r="W38" s="24"/>
+      <c r="X38" s="25"/>
+      <c r="Y38" s="25"/>
+      <c r="Z38" s="26"/>
+    </row>
+    <row r="39" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B39" s="80"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="42"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="41"/>
+      <c r="I39" s="42"/>
+      <c r="J39" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="K39" s="41"/>
+      <c r="L39" s="42"/>
+      <c r="M39" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="N39" s="72"/>
+      <c r="O39" s="72"/>
+      <c r="P39" s="73"/>
+      <c r="Q39" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="R39" s="63"/>
+      <c r="S39" s="64"/>
+      <c r="T39" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="U39" s="41"/>
+      <c r="V39" s="42"/>
+      <c r="W39" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X39" s="41"/>
+      <c r="Y39" s="41"/>
+      <c r="Z39" s="42"/>
+    </row>
+    <row r="40" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B40" s="81"/>
+      <c r="C40" s="81"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="44"/>
+      <c r="I40" s="45"/>
+      <c r="J40" s="43"/>
+      <c r="K40" s="44"/>
+      <c r="L40" s="45"/>
+      <c r="M40" s="74"/>
+      <c r="N40" s="75"/>
+      <c r="O40" s="75"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="65"/>
+      <c r="R40" s="66"/>
+      <c r="S40" s="67"/>
+      <c r="T40" s="43"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="45"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="44"/>
+      <c r="Y40" s="44"/>
+      <c r="Z40" s="45"/>
+    </row>
+    <row r="41" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B41" s="81"/>
+      <c r="C41" s="81"/>
+      <c r="D41" s="43"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="43"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="44"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="43"/>
+      <c r="K41" s="44"/>
+      <c r="L41" s="45"/>
+      <c r="M41" s="74"/>
+      <c r="N41" s="75"/>
+      <c r="O41" s="75"/>
+      <c r="P41" s="76"/>
+      <c r="Q41" s="65"/>
+      <c r="R41" s="66"/>
+      <c r="S41" s="67"/>
+      <c r="T41" s="43"/>
+      <c r="U41" s="44"/>
+      <c r="V41" s="45"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="44"/>
+      <c r="Y41" s="44"/>
+      <c r="Z41" s="45"/>
+    </row>
+    <row r="42" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="46"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="48"/>
+      <c r="M42" s="77"/>
+      <c r="N42" s="78"/>
+      <c r="O42" s="78"/>
+      <c r="P42" s="79"/>
+      <c r="Q42" s="68"/>
+      <c r="R42" s="69"/>
+      <c r="S42" s="70"/>
+      <c r="T42" s="46"/>
+      <c r="U42" s="47"/>
+      <c r="V42" s="48"/>
+      <c r="W42" s="46"/>
+      <c r="X42" s="47"/>
+      <c r="Y42" s="47"/>
+      <c r="Z42" s="48"/>
+    </row>
+    <row r="43" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="49" t="s">
+        <v>76</v>
+      </c>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="R43" s="38"/>
+      <c r="S43" s="38"/>
+      <c r="T43" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="U43" s="38"/>
+      <c r="V43" s="38"/>
+      <c r="W43" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="X43" s="19"/>
+      <c r="Y43" s="19"/>
+      <c r="Z43" s="20"/>
+    </row>
+    <row r="44" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="38"/>
+      <c r="T44" s="38"/>
+      <c r="U44" s="38"/>
+      <c r="V44" s="38"/>
+      <c r="W44" s="21"/>
+      <c r="X44" s="22"/>
+      <c r="Y44" s="22"/>
+      <c r="Z44" s="23"/>
+    </row>
+    <row r="45" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="38"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="38"/>
+      <c r="S45" s="38"/>
+      <c r="T45" s="38"/>
+      <c r="U45" s="38"/>
+      <c r="V45" s="38"/>
+      <c r="W45" s="21"/>
+      <c r="X45" s="22"/>
+      <c r="Y45" s="22"/>
+      <c r="Z45" s="23"/>
+    </row>
+    <row r="46" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="38"/>
+      <c r="N46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="38"/>
+      <c r="S46" s="38"/>
+      <c r="T46" s="38"/>
+      <c r="U46" s="38"/>
+      <c r="V46" s="38"/>
+      <c r="W46" s="24"/>
+      <c r="X46" s="25"/>
+      <c r="Y46" s="25"/>
+      <c r="Z46" s="26"/>
+    </row>
+    <row r="47" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="50" t="s">
+        <v>72</v>
+      </c>
+      <c r="N47" s="37"/>
+      <c r="O47" s="37"/>
+      <c r="P47" s="37"/>
+      <c r="Q47" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="R47" s="37"/>
+      <c r="S47" s="37"/>
+      <c r="T47" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="U47" s="36"/>
+      <c r="V47" s="36"/>
+      <c r="W47" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="X47" s="41"/>
+      <c r="Y47" s="41"/>
+      <c r="Z47" s="42"/>
+    </row>
+    <row r="48" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B48" s="36"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="37"/>
+      <c r="N48" s="37"/>
+      <c r="O48" s="37"/>
+      <c r="P48" s="37"/>
+      <c r="Q48" s="37"/>
+      <c r="R48" s="37"/>
+      <c r="S48" s="37"/>
+      <c r="T48" s="36"/>
+      <c r="U48" s="36"/>
+      <c r="V48" s="36"/>
+      <c r="W48" s="43"/>
+      <c r="X48" s="44"/>
+      <c r="Y48" s="44"/>
+      <c r="Z48" s="45"/>
+    </row>
+    <row r="49" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B49" s="36"/>
+      <c r="C49" s="36"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="36"/>
+      <c r="I49" s="36"/>
+      <c r="J49" s="36"/>
+      <c r="K49" s="36"/>
+      <c r="L49" s="36"/>
+      <c r="M49" s="37"/>
+      <c r="N49" s="37"/>
+      <c r="O49" s="37"/>
+      <c r="P49" s="37"/>
+      <c r="Q49" s="37"/>
+      <c r="R49" s="37"/>
+      <c r="S49" s="37"/>
+      <c r="T49" s="36"/>
+      <c r="U49" s="36"/>
+      <c r="V49" s="36"/>
+      <c r="W49" s="43"/>
+      <c r="X49" s="44"/>
+      <c r="Y49" s="44"/>
+      <c r="Z49" s="45"/>
+    </row>
+    <row r="50" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B50" s="36"/>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="36"/>
+      <c r="J50" s="36"/>
+      <c r="K50" s="36"/>
+      <c r="L50" s="36"/>
+      <c r="M50" s="37"/>
+      <c r="N50" s="37"/>
+      <c r="O50" s="37"/>
+      <c r="P50" s="37"/>
+      <c r="Q50" s="37"/>
+      <c r="R50" s="37"/>
+      <c r="S50" s="37"/>
+      <c r="T50" s="36"/>
+      <c r="U50" s="36"/>
+      <c r="V50" s="36"/>
+      <c r="W50" s="46"/>
+      <c r="X50" s="47"/>
+      <c r="Y50" s="47"/>
+      <c r="Z50" s="48"/>
+    </row>
+  </sheetData>
+  <mergeCells count="116">
+    <mergeCell ref="Q47:S50"/>
+    <mergeCell ref="T47:V50"/>
+    <mergeCell ref="W47:Z50"/>
+    <mergeCell ref="B47:B50"/>
+    <mergeCell ref="C47:C50"/>
+    <mergeCell ref="D47:E50"/>
+    <mergeCell ref="F47:I50"/>
+    <mergeCell ref="J47:L50"/>
+    <mergeCell ref="M47:P50"/>
+    <mergeCell ref="W39:Z42"/>
+    <mergeCell ref="B43:B46"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="F43:I46"/>
+    <mergeCell ref="J43:L46"/>
+    <mergeCell ref="M43:P46"/>
+    <mergeCell ref="Q43:S46"/>
+    <mergeCell ref="T43:V46"/>
+    <mergeCell ref="W43:Z46"/>
+    <mergeCell ref="T35:V38"/>
+    <mergeCell ref="W35:Z38"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="D39:E42"/>
+    <mergeCell ref="F39:I42"/>
+    <mergeCell ref="J39:L42"/>
+    <mergeCell ref="M39:P42"/>
+    <mergeCell ref="Q39:S42"/>
+    <mergeCell ref="T39:V42"/>
+    <mergeCell ref="Q31:S34"/>
+    <mergeCell ref="T31:V34"/>
+    <mergeCell ref="W31:Z34"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="D35:E38"/>
+    <mergeCell ref="F35:I38"/>
+    <mergeCell ref="J35:L38"/>
+    <mergeCell ref="M35:P38"/>
+    <mergeCell ref="Q35:S38"/>
+    <mergeCell ref="T27:V30"/>
+    <mergeCell ref="W27:X30"/>
+    <mergeCell ref="Y27:Z30"/>
+    <mergeCell ref="B31:B34"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D31:E34"/>
+    <mergeCell ref="F31:I34"/>
+    <mergeCell ref="J31:L34"/>
+    <mergeCell ref="M31:P34"/>
+    <mergeCell ref="Q23:S26"/>
+    <mergeCell ref="T23:V26"/>
+    <mergeCell ref="W23:Z26"/>
+    <mergeCell ref="B27:B30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="D27:E30"/>
+    <mergeCell ref="F27:I30"/>
+    <mergeCell ref="J27:L30"/>
+    <mergeCell ref="M27:P30"/>
+    <mergeCell ref="Q27:S30"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="D23:E26"/>
+    <mergeCell ref="F23:I26"/>
+    <mergeCell ref="J23:L26"/>
+    <mergeCell ref="M23:P26"/>
+    <mergeCell ref="W15:Z18"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="C19:C22"/>
+    <mergeCell ref="D19:E22"/>
+    <mergeCell ref="F19:I22"/>
+    <mergeCell ref="J19:L22"/>
+    <mergeCell ref="M19:P22"/>
+    <mergeCell ref="Q19:S22"/>
+    <mergeCell ref="T19:V22"/>
+    <mergeCell ref="W19:Z22"/>
+    <mergeCell ref="T11:V14"/>
+    <mergeCell ref="W11:Z14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="C15:C18"/>
+    <mergeCell ref="D15:E18"/>
+    <mergeCell ref="F15:I18"/>
+    <mergeCell ref="J15:L18"/>
+    <mergeCell ref="M15:P18"/>
+    <mergeCell ref="Q15:S18"/>
+    <mergeCell ref="T15:V18"/>
+    <mergeCell ref="Q7:S10"/>
+    <mergeCell ref="T7:V10"/>
+    <mergeCell ref="W7:Z10"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="D11:E14"/>
+    <mergeCell ref="F11:I14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="M11:P14"/>
+    <mergeCell ref="Q11:S14"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="F7:I10"/>
+    <mergeCell ref="J7:L10"/>
+    <mergeCell ref="M7:P10"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="D3:E6"/>
+    <mergeCell ref="F3:I6"/>
+    <mergeCell ref="J3:L6"/>
+    <mergeCell ref="M3:P6"/>
+    <mergeCell ref="Q3:S6"/>
+    <mergeCell ref="T3:V6"/>
+    <mergeCell ref="W3:X6"/>
+    <mergeCell ref="Y3:Z6"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:P2"/>
+    <mergeCell ref="Q2:S2"/>
+    <mergeCell ref="T2:V2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="M7" r:id="rId1" display="https://coffeeshop2023.netlify.app/sign-up"/>
+    <hyperlink ref="M31" r:id="rId2" display="https://coffeeshop2023.netlify.app/sign-up"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>